<commit_message>
group leader feedback and edits
</commit_message>
<xml_diff>
--- a/temp/pages/StructureDefinition-alabama-consent-profile.xlsx
+++ b/temp/pages/StructureDefinition-alabama-consent-profile.xlsx
@@ -24,13 +24,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://gitlab.mitre.org/awatson/us-state-profiles/StructureDefinition/alabama-consent-profile</t>
+    <t>https://github.com/awatson1978/us-state-profiles/StructureDefinition/alabama-consent-profile</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>0.5.0</t>
+    <t>0.6.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-29T13:10:12-06:00</t>
+    <t>2024-05-12T21:17:02-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -790,7 +790,7 @@
     <t>Might be a unique identifier of a policy set in XACML, or other rules engine.</t>
   </si>
   <si>
-    <t>https://gitlab.mitre.org/awatson/us-state-profiles/ValueSet/ConsentExchangePolicies</t>
+    <t>https://github.com/awatson1978/us-state-profiles/ValueSet/ConsentExchangePolicies</t>
   </si>
   <si>
     <t>Consent.verification</t>
@@ -1439,7 +1439,7 @@
     <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="121.84765625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="78.5390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="79.38671875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="18.84765625" customWidth="true" bestFit="true"/>

</xml_diff>